<commit_message>
DP: ad-hoc-forecast-with-changing-taz - status_exists_for_control.py - change lines 3-5 in inputs_outputs of current forecast basic excel
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">location</t>
   </si>
   <si>
-    <t xml:space="preserve">מיקום תוכנה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W:\Data\Forecast\Tools\creat_forecast_ad_hoc</t>
+    <t xml:space="preserve">מיקום תוכנת תחזית בסיס</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast\create_forecast_basic\current</t>
   </si>
   <si>
     <t xml:space="preserve">מיקום לקוח</t>
@@ -132,16 +132,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,93 +169,93 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>240129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1"/>
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
DP: ad-hoc-forecast-with-changing-taz - run_basic_from_ad_hoc, fox ad-hoc bugs, and testing
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">v_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מיקום פלט תחזית בסיס לפי גירסא</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,6 +153,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -169,7 +179,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,9 +228,13 @@
         <v>240129</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
DP: ad-hoc-forecast-with-changing-taz - main.py - fix paths bugs
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">מיקום תוכנת תחזית בסיס</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast\create_forecast_basic\current</t>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current</t>
   </si>
   <si>
     <t xml:space="preserve">מיקום לקוח</t>
@@ -155,7 +155,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,7 +179,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
DP: change output_inputs ad_hoc file
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA66238-17EC-49F2-A095-0D3FD2171604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613C11AA-9700-45D0-B757-8CC43CF066CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>discription</t>
   </si>
@@ -33,7 +33,7 @@
     <t>location</t>
   </si>
   <si>
-    <t>מיקום תוכנה</t>
+    <t>מיקום תוכנת תחזית בסיס</t>
   </si>
   <si>
     <t>מיקום לקוח</t>
@@ -45,13 +45,19 @@
     <t>v_date</t>
   </si>
   <si>
+    <t>מיקום פלט תחזית בסיס לפי גירסא</t>
+  </si>
+  <si>
+    <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
+  </si>
+  <si>
+    <t>W:\Projects\תכניות אב עירוניות\136_תכנית_אב_מודיעין_עלית\קבצי עבודה\תחזיות_דמוגרפיות</t>
+  </si>
+  <si>
     <t>with_project</t>
   </si>
   <si>
-    <t>W:\Projects\תכניות אב עירוניות\136_תכנית_אב_מודיעין_עלית\קבצי עבודה\תחזיות_דמוגרפיות</t>
-  </si>
-  <si>
-    <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc</t>
+    <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
 </sst>
 </file>
@@ -69,7 +75,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא של Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -126,39 +132,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +216,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -262,7 +268,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -321,13 +327,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -336,6 +335,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -400,11 +406,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,7 +441,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -437,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -445,7 +471,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -453,7 +479,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -464,9 +490,13 @@
         <v>240229</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
DP: create_forecast_ad_hoc - make promoteres dynamic
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -31,19 +31,19 @@
     <t xml:space="preserve">מיקום תוכנת תחזית בסיס</t>
   </si>
   <si>
-    <t xml:space="preserve">W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current</t>
   </si>
   <si>
     <t xml:space="preserve">מיקום לקוח</t>
   </si>
   <si>
-    <t xml:space="preserve">W:\Projects\תכניות אב עירוניות\136_תכנית_אב_מודיעין_עלית\קבצי עבודה\תחזיות_דמוגרפיות</t>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת</t>
   </si>
   <si>
     <t xml:space="preserve">שם תרחיש (forecast_version)</t>
   </si>
   <si>
-    <t xml:space="preserve">with_project</t>
+    <t xml:space="preserve">without_project</t>
   </si>
   <si>
     <t xml:space="preserve">v_date</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">מיקום פלט תחזית בסיס לפי גירסא</t>
   </si>
   <si>
-    <t xml:space="preserve">W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
   </si>
   <si>
     <t xml:space="preserve">מספר גירסא</t>
@@ -141,16 +141,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,101 +178,101 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>240229</v>
+      <c r="B5" s="2" t="n">
+        <v>240129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1"/>
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
EL: input_output ad hoc bug fix
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613C11AA-9700-45D0-B757-8CC43CF066CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14434C20-5576-48C9-8FDA-FEE13843D443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
   </si>
   <si>
-    <t>W:\Projects\תכניות אב עירוניות\136_תכנית_אב_מודיעין_עלית\קבצי עבודה\תחזיות_דמוגרפיות</t>
-  </si>
-  <si>
     <t>with_project</t>
   </si>
   <si>
     <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+  </si>
+  <si>
+    <t>W:\Projects\בהת\135_סטריפ_דרך_חברון\קבצי עבודה\תחזיות_דמוגרפיות</t>
   </si>
 </sst>
 </file>
@@ -441,16 +441,16 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="81.21875" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="81.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -466,71 +466,71 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>240229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>240530</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GK: saveing after EL run code for gilo ad hoc
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EEE7BF-AE8B-436C-B1B8-109BD736F64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9C47B2-3CAD-4C38-AA04-70B8D6E87A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="3420" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -57,13 +57,13 @@
     <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
   <si>
-    <t>240410_with_poten</t>
-  </si>
-  <si>
-    <t>W:\Projects\תכניות מרחביות\בדיקה_מרחבית_קטמונים_123\קבצי עבודה\תחזיות_דמוגרפיות</t>
-  </si>
-  <si>
-    <t>max</t>
+    <t>240818_with_poten</t>
+  </si>
+  <si>
+    <t>W:\Projects\תכניות מרחביות\בדיקה מרחבית גילה\קבצי עבודה\תחזיות_דמוגרפיות</t>
+  </si>
+  <si>
+    <t>realy</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
GK fix background files for yecotial plan
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252AD4B7-BF27-41A9-A89B-F622016FC819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7680E6-812A-48E2-A04E-9C824306A117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>discription</t>
   </si>
@@ -54,16 +54,13 @@
     <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
   </si>
   <si>
-    <t>W:\Projects\תכניות מרחביות\בדיקה מרחבית גילה\קבצי עבודה\תחזיות_דמוגרפיות</t>
-  </si>
-  <si>
     <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
   <si>
-    <t>240923_with_poten</t>
-  </si>
-  <si>
-    <t>with_project_muni</t>
+    <t>W:\Projects\בהת\176 יקותיאל אדם\קבצי עבודה\תחזיות_דמוגרפיות</t>
+  </si>
+  <si>
+    <t>with_project</t>
   </si>
 </sst>
 </file>
@@ -447,7 +444,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -477,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
@@ -485,15 +482,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
+      <c r="B5" s="1">
+        <v>240929</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -501,7 +498,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
GK: fix bug with factor that were double,fixed urben layer
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7680E6-812A-48E2-A04E-9C824306A117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D80A65-2D3E-4B4D-88D8-544D7FE45992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25395" yWindow="3630" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
     <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
   <si>
-    <t>W:\Projects\בהת\176 יקותיאל אדם\קבצי עבודה\תחזיות_דמוגרפיות</t>
-  </si>
-  <si>
-    <t>with_project</t>
+    <t>W:\Projects\בהת\154_בית_שמש_מתאר_דרום\קבצי עבודה\תחזיות_דמוגרפיות</t>
+  </si>
+  <si>
+    <t>full_realization_BS</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>240929</v>
+        <v>241028</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
DP - create_forecast_ad_hoc - main & status_exists_for_control - fix inputs_outputs.xlsx & change run_create_forecast_basic to run_basic
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">מיקום לקוח</t>
   </si>
   <si>
-    <t xml:space="preserve">W:\Projects\בהת\135_סטריפ_דרך_חברון\קבצי עבודה\תחזיות_דמוגרפיות</t>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת</t>
   </si>
   <si>
     <t xml:space="preserve">שם תרחיש (forecast_version)</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">מיקום פלט תחזית בסיס לפי גירסא</t>
   </si>
   <si>
-    <t xml:space="preserve">W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_by_version\V4</t>
   </si>
 </sst>
 </file>
@@ -132,16 +132,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,89 +169,89 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>240530</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
DP - create_forecast_ad_hoc - update ad_hoc
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -28,6 +28,12 @@
     <t xml:space="preserve">location</t>
   </si>
   <si>
+    <t xml:space="preserve">מיקום תוכנת תחזית בסיס</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current</t>
+  </si>
+  <si>
     <t xml:space="preserve">מיקום לקוח</t>
   </si>
   <si>
@@ -37,16 +43,22 @@
     <t xml:space="preserve">שם תרחיש (forecast_version)</t>
   </si>
   <si>
-    <t xml:space="preserve">with_project</t>
+    <t xml:space="preserve">realy</t>
   </si>
   <si>
     <t xml:space="preserve">v_date</t>
   </si>
   <si>
+    <t xml:space="preserve">240818_with_poten</t>
+  </si>
+  <si>
     <t xml:space="preserve">מיקום פלט תחזית בסיס לפי גירסא</t>
   </si>
   <si>
     <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_by_version\V4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מספר גירסא</t>
   </si>
 </sst>
 </file>
@@ -132,20 +144,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,94 +174,105 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>240530</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
DP - create_forecast_ad_hoc - setup main.ipynb
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
   <si>
     <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מיקום תוכנת תחזית בסיס</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current</t>
   </si>
   <si>
     <t xml:space="preserve">מיקום לקוח</t>
@@ -144,16 +138,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,105 +172,98 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
+      <c r="B6" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1"/>
-    </row>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
DP - create_forecast_ad_hoc - main.ipynb - run all and cleanup
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -37,13 +37,10 @@
     <t xml:space="preserve">שם תרחיש (forecast_version)</t>
   </si>
   <si>
-    <t xml:space="preserve">realy</t>
+    <t xml:space="preserve">without_project</t>
   </si>
   <si>
     <t xml:space="preserve">v_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">240818_with_poten</t>
   </si>
   <si>
     <t xml:space="preserve">מיקום פלט תחזית בסיס לפי גירסא</t>
@@ -175,7 +172,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -200,7 +197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -208,25 +205,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="2" t="n">
+        <v>240129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
GK: fix mixup do to dropgeo in wrong place
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/inputs_outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D80A65-2D3E-4B4D-88D8-544D7FE45992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45FFEF7-60E4-48BF-A07A-B458DBDFDAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25395" yWindow="3630" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="3030" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
     <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
   <si>
-    <t>W:\Projects\בהת\154_בית_שמש_מתאר_דרום\קבצי עבודה\תחזיות_דמוגרפיות</t>
-  </si>
-  <si>
-    <t>full_realization_BS</t>
+    <t>with_project</t>
+  </si>
+  <si>
+    <t>W:\Projects\בהת\175 תכנית מתאר קמפוס גבעת רם\קבצי עבודה\תחזיות_דמוגרפיות</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>241028</v>
+        <v>241209</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>